<commit_message>
updated  matrix diagram for the database
</commit_message>
<xml_diff>
--- a/Matrix dig wbs monitor oude versie.xlsx
+++ b/Matrix dig wbs monitor oude versie.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damien\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wbsMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>project</t>
   </si>
@@ -39,12 +42,15 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,8 +86,36 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -169,6 +203,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -204,6 +255,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -359,7 +427,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,18 +456,33 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" t="s">
         <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>

</xml_diff>